<commit_message>
BOM DCDC actualizada para 1ra produccion SETI 500uds
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_DCDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\TEAMDR~1\JRODRI~1\Repositorios\01.Rover\02.HARDWARE\V2-ROVER-1K\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD14321D-3B45-4FF3-89FE-A1D3144BE7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0E483F-3A92-7C4C-BA62-FE20E8A499AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23115" yWindow="3255" windowWidth="36300" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22100" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_DCDC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
   <si>
     <t>Qty</t>
   </si>
@@ -55,18 +55,9 @@
     <t>R4, R15, R16</t>
   </si>
   <si>
-    <t>100mR</t>
-  </si>
-  <si>
     <t>RSENSE</t>
   </si>
   <si>
-    <t>100n</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
     <t>2.2uH - 74437346022</t>
   </si>
   <si>
-    <t>INDM7366X500</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -190,9 +178,6 @@
     <t>B520C-13-F</t>
   </si>
   <si>
-    <t>DIOM7959X250N</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -217,9 +202,6 @@
     <t>TPS55330RTET</t>
   </si>
   <si>
-    <t>RTE16_1P66X1P66_TEX</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -274,9 +256,6 @@
     <t>SMD 1210</t>
   </si>
   <si>
-    <t>SOT65</t>
-  </si>
-  <si>
     <t>SOT-23-5</t>
   </si>
   <si>
@@ -338,12 +317,6 @@
   </si>
   <si>
     <t>DELETED</t>
-  </si>
-  <si>
-    <t>270pF</t>
-  </si>
-  <si>
-    <t>1uF</t>
   </si>
   <si>
     <t>8-powerWDFN</t>
@@ -359,9 +332,6 @@
   </si>
   <si>
     <t>C7</t>
-  </si>
-  <si>
-    <t>220pF</t>
   </si>
   <si>
     <t>C9</t>
@@ -406,6 +376,63 @@
 Se crea la posicion 35 con el part R7 y valor 4k3
 Se crea la posicion 36 con los part R14 y R17, y valor 100R
 Se crea la posicion 37 con los part R18 y valor 0R.</t>
+  </si>
+  <si>
+    <t>5-ene-2023</t>
+  </si>
+  <si>
+    <t>1.0uF, 16V, X7R</t>
+  </si>
+  <si>
+    <t>100nF, 25V, X7R o X5R</t>
+  </si>
+  <si>
+    <t>100pF, 25V, C0G</t>
+  </si>
+  <si>
+    <t>10uF, 12V, X7R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/nexperia-usa-inc/BAT54SW-115/763219?s=N4IgTCBcDaIEIEEAqBWALAZQOoBoCMeKIAugL5A</t>
+  </si>
+  <si>
+    <t>Corregido valor de C22 (100pf. antes 220pf). Corregido package D1</t>
+  </si>
+  <si>
+    <t>DO214</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/diodes-incorporated/B520C-13-F/806535?s=N4IgTCBcDaIEIFYwAYDCBaAjAZnQMRAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/würth-elektronik/74437346022/2790921?s=N4IgTCBcDaIOwBYEGY7IQNgAxggXQF8g</t>
+  </si>
+  <si>
+    <t>7.3 x 6.6 x 3.1mm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/onsemi/NVTFS9D6P04M8LTAG/11592842?s=N4IgTCBcDaIHIDUAqAxAygTgCIDYAKADACwCyAHADJICCA4iALoC%2BQA</t>
+  </si>
+  <si>
+    <t>SMD 1206</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/ohmite/KDV12FR100ET/10476508</t>
+  </si>
+  <si>
+    <t>100mR, 1%, 1/2W, 100ppm - KDV12FR100ET</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/microchip-technology/MCP6071T-E-OT/2614948</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/texas-instruments/TPS55330RTET/4212800?s=N4IgTCBcDaICoAUDKBWFBmdAGASnAonCALoC%2BQA</t>
+  </si>
+  <si>
+    <t>16-WFQFN</t>
+  </si>
+  <si>
+    <t>220pF, 16V, C0G</t>
   </si>
 </sst>
 </file>
@@ -1143,194 +1170,69 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="7">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -1409,14 +1311,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:J43" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:J43" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A6:J43" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J38">
     <sortCondition ref="D6:D38"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
-    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{AB092131-4167-465E-A2DF-04757A83F427}" name="NEW" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{958FBBFD-8FA4-4642-8441-E180A56F96F0}" name="Qty"/>
     <tableColumn id="3" xr3:uid="{FBAE2CFA-77A4-45AD-9266-0EFC588D4B64}" name="Part"/>
     <tableColumn id="4" xr3:uid="{FB9BFB6E-6495-468E-802B-025835AD898D}" name="Value"/>
@@ -1431,7 +1333,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1729,64 +1631,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.4">
+        <f>MAX(_HISTORY!A4:A55)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="26" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="26" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="22"/>
     </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
@@ -1798,545 +1701,557 @@
         <v>3</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -2348,332 +2263,341 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F35" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="F36" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="J36" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F37" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F39" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F40" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G41" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E42" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E43" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F43" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G43" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2681,20 +2605,29 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B43">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J16" r:id="rId1" xr:uid="{4EF74C74-5599-D341-A184-4262A41DCCB8}"/>
+    <hyperlink ref="J17" r:id="rId2" xr:uid="{25F4A353-B9E3-8846-9826-52724C670B5F}"/>
+    <hyperlink ref="J18" r:id="rId3" xr:uid="{B4F6A03A-A5DE-9B42-92BD-39D8294FBCE8}"/>
+    <hyperlink ref="J19" r:id="rId4" xr:uid="{9CE05E9A-D9C3-4A45-8F2A-3443DA782029}"/>
+    <hyperlink ref="J36" r:id="rId5" xr:uid="{C813FBCD-BBA9-7C41-B5BA-B64FA046AB8A}"/>
+    <hyperlink ref="J37" r:id="rId6" xr:uid="{0374EAFF-2FDA-AA4E-A136-EB33DA6E9CFA}"/>
+    <hyperlink ref="J38" r:id="rId7" xr:uid="{11C11D1A-BC77-584C-84B8-7A63B99051B2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2703,35 +2636,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5396D425-0A04-B64D-B9F7-D3F9797B3C5D}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2739,13 +2672,13 @@
         <v>44874</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2753,13 +2686,13 @@
         <v>44880</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2767,14 +2700,25 @@
         <v>44922</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2789,70 +2733,70 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>28805</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C9" s="11"/>
     </row>

</xml_diff>

<commit_message>
1ra produccion seti 500uds
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_DCDC.xlsx
+++ b/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_DCDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0E483F-3A92-7C4C-BA62-FE20E8A499AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D615FFB-8104-2D47-A3B6-93A983F86D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22100" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="130">
   <si>
     <t>Qty</t>
   </si>
@@ -434,6 +434,9 @@
   <si>
     <t>220pF, 16V, C0G</t>
   </si>
+  <si>
+    <t>SI</t>
+  </si>
 </sst>
 </file>
 
@@ -665,7 +668,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +875,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,7 +1120,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1158,6 +1167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1170,7 +1180,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1631,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1665,12 +1677,12 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="26" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
@@ -1957,7 +1969,7 @@
       <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="20" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1983,7 +1995,7 @@
       <c r="G17" t="s">
         <v>117</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="J17" s="20" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2009,7 +2021,7 @@
       <c r="G18" t="s">
         <v>120</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="20" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2035,7 +2047,7 @@
       <c r="G19" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="20" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2411,8 +2423,8 @@
       <c r="A36">
         <v>30</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>75</v>
+      <c r="B36" s="25" t="s">
+        <v>129</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2429,7 +2441,7 @@
       <c r="G36" t="s">
         <v>122</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="J36" s="20" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2455,7 +2467,7 @@
       <c r="G37" t="s">
         <v>73</v>
       </c>
-      <c r="J37" s="24" t="s">
+      <c r="J37" s="20" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2481,7 +2493,7 @@
       <c r="G38" t="s">
         <v>127</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="J38" s="20" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2736,11 +2748,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">

</xml_diff>